<commit_message>
updated excel sheets for ado
</commit_message>
<xml_diff>
--- a/ado-bitbucket/azure-to-bitbucket.xlsx
+++ b/ado-bitbucket/azure-to-bitbucket.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varsharma\Desktop\version control excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abharamagoudar\Desktop\api\github\SCM-Migration-DEMO\ado-bitbucket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46048007-F098-4E82-B128-5A3A8BABA4F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5DCBCC-7763-44C7-8E5C-EC5B628EA16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1452" yWindow="5964" windowWidth="19536" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>sr</t>
   </si>
@@ -33,12 +33,6 @@
     <t>azure_namespace</t>
   </si>
   <si>
-    <t>devops-TEKsystems/test</t>
-  </si>
-  <si>
-    <t>Sync_CodeCommit</t>
-  </si>
-  <si>
     <t>bitbucket_workspace_id</t>
   </si>
   <si>
@@ -48,13 +42,28 @@
     <t>repo_to_import</t>
   </si>
   <si>
-    <t>varun160799</t>
-  </si>
-  <si>
-    <t>TES</t>
-  </si>
-  <si>
-    <t>service_catalog</t>
+    <t>repo-migartion/git-project</t>
+  </si>
+  <si>
+    <t>app-n-pak</t>
+  </si>
+  <si>
+    <t>ALMAtasks</t>
+  </si>
+  <si>
+    <t>CASAshell</t>
+  </si>
+  <si>
+    <t>casa-build-utils</t>
+  </si>
+  <si>
+    <t>CASAplotserver</t>
+  </si>
+  <si>
+    <t>anilsb06</t>
+  </si>
+  <si>
+    <t>REP</t>
   </si>
 </sst>
 </file>
@@ -381,20 +390,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E2" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-    <col min="4" max="5" width="25.21875" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="5" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,47 +411,98 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>